<commit_message>
add a few cities and Kern county in the template
</commit_message>
<xml_diff>
--- a/server/api/trucking-company/templates/BDL-Rates.xlsx
+++ b/server/api/trucking-company/templates/BDL-Rates.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17300" yWindow="1280" windowWidth="34480" windowHeight="24800" tabRatio="500"/>
+    <workbookView xWindow="10860" yWindow="1480" windowWidth="31560" windowHeight="23340" tabRatio="500" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="Santa Barbara" sheetId="7" r:id="rId7"/>
     <sheet name="San Diego" sheetId="8" r:id="rId8"/>
     <sheet name="San Luis Obispo" sheetId="9" r:id="rId9"/>
+    <sheet name="Kern County" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5484" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5622" uniqueCount="462">
   <si>
     <t>City</t>
   </si>
@@ -1293,6 +1294,129 @@
   </si>
   <si>
     <t>Morono Valley</t>
+  </si>
+  <si>
+    <t>Kern</t>
+  </si>
+  <si>
+    <t>Johannesburg</t>
+  </si>
+  <si>
+    <t>Boron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pine Mountain Club </t>
+  </si>
+  <si>
+    <t>Bakersfield</t>
+  </si>
+  <si>
+    <t>Woody</t>
+  </si>
+  <si>
+    <t>Ridgecrest</t>
+  </si>
+  <si>
+    <t>Randsburg</t>
+  </si>
+  <si>
+    <t>Edison</t>
+  </si>
+  <si>
+    <t>Red Mountain</t>
+  </si>
+  <si>
+    <t>Caliente</t>
+  </si>
+  <si>
+    <t>Tehachapi</t>
+  </si>
+  <si>
+    <t>Cantil</t>
+  </si>
+  <si>
+    <t>Rosamond</t>
+  </si>
+  <si>
+    <t>Keene</t>
+  </si>
+  <si>
+    <t>Fellows</t>
+  </si>
+  <si>
+    <t>Edwards</t>
+  </si>
+  <si>
+    <t>Mc Kittrick</t>
+  </si>
+  <si>
+    <t>Frazier Park</t>
+  </si>
+  <si>
+    <t>Buttonwillow</t>
+  </si>
+  <si>
+    <t>Delano</t>
+  </si>
+  <si>
+    <t>Maricopa</t>
+  </si>
+  <si>
+    <t>Onyx</t>
+  </si>
+  <si>
+    <t>Inyokern</t>
+  </si>
+  <si>
+    <t>Lake Isabella</t>
+  </si>
+  <si>
+    <t>Kernville</t>
+  </si>
+  <si>
+    <t>Lamont</t>
+  </si>
+  <si>
+    <t>Arvin</t>
+  </si>
+  <si>
+    <t>Mc Farland</t>
+  </si>
+  <si>
+    <t>Bodfish</t>
+  </si>
+  <si>
+    <t>Lost Hills</t>
+  </si>
+  <si>
+    <t>Lebec</t>
+  </si>
+  <si>
+    <t>Glennville</t>
+  </si>
+  <si>
+    <t>Wasco</t>
+  </si>
+  <si>
+    <t>Tupman</t>
+  </si>
+  <si>
+    <t>California City</t>
+  </si>
+  <si>
+    <t>Wofford Heights</t>
+  </si>
+  <si>
+    <t>Weldon</t>
+  </si>
+  <si>
+    <t>Mojave</t>
+  </si>
+  <si>
+    <t>Taft</t>
+  </si>
+  <si>
+    <t>Shafter</t>
   </si>
 </sst>
 </file>
@@ -1825,7 +1949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1190"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -17110,6 +17234,995 @@
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="39" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16">
+      <c r="A1" s="2">
+        <v>93528</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D1" s="2">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16">
+      <c r="A2" s="2">
+        <v>93516</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D2" s="2">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16">
+      <c r="A3" s="2">
+        <v>93222</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D3" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16">
+      <c r="A4" s="2">
+        <v>93313</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D4" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16">
+      <c r="A5" s="2">
+        <v>93383</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D5" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16">
+      <c r="A6" s="2">
+        <v>93301</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D6" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16">
+      <c r="A7" s="2">
+        <v>93596</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D7" s="2">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16">
+      <c r="A8" s="2">
+        <v>93384</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D8" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16">
+      <c r="A9" s="2">
+        <v>93287</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D9" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16">
+      <c r="A10" s="2">
+        <v>93308</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D10" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16">
+      <c r="A11" s="2">
+        <v>93309</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D11" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16">
+      <c r="A12" s="2">
+        <v>93556</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D12" s="2">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16">
+      <c r="A13" s="2">
+        <v>93385</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D13" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16">
+      <c r="A14" s="2">
+        <v>93554</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D14" s="2">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16">
+      <c r="A15" s="2">
+        <v>93220</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D15" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16">
+      <c r="A16" s="2">
+        <v>93555</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D16" s="2">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16">
+      <c r="A17" s="2">
+        <v>93302</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D17" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16">
+      <c r="A18" s="2">
+        <v>93312</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D18" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16">
+      <c r="A19" s="2">
+        <v>93311</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D19" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16">
+      <c r="A20" s="2">
+        <v>93558</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D20" s="2">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16">
+      <c r="A21" s="2">
+        <v>93518</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D21" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16">
+      <c r="A22" s="2">
+        <v>93307</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D22" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16">
+      <c r="A23" s="2">
+        <v>93561</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D23" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16">
+      <c r="A24" s="2">
+        <v>93519</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D24" s="2">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16">
+      <c r="A25" s="2">
+        <v>93560</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D25" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16">
+      <c r="A26" s="2">
+        <v>93304</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D26" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16">
+      <c r="A27" s="2">
+        <v>93380</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D27" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16">
+      <c r="A28" s="2">
+        <v>93303</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D28" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16">
+      <c r="A29" s="2">
+        <v>93581</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D29" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16">
+      <c r="A30" s="2">
+        <v>93531</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D30" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16">
+      <c r="A31" s="2">
+        <v>93314</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D31" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="16">
+      <c r="A32" s="2">
+        <v>93305</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D32" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16">
+      <c r="A33" s="2">
+        <v>93306</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D33" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16">
+      <c r="A34" s="2">
+        <v>93224</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D34" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16">
+      <c r="A35" s="2">
+        <v>93523</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D35" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="16">
+      <c r="A36" s="2">
+        <v>93251</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D36" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16">
+      <c r="A37" s="2">
+        <v>93225</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D37" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16">
+      <c r="A38" s="2">
+        <v>93206</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D38" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="16">
+      <c r="A39" s="2">
+        <v>93215</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D39" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="16">
+      <c r="A40" s="2">
+        <v>93252</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D40" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="16">
+      <c r="A41" s="2">
+        <v>93255</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D41" s="2">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="16">
+      <c r="A42" s="2">
+        <v>93527</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D42" s="2">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="16">
+      <c r="A43" s="2">
+        <v>93389</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D43" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="16">
+      <c r="A44" s="2">
+        <v>93222</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D44" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="16">
+      <c r="A45" s="2">
+        <v>93240</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D45" s="2">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="16">
+      <c r="A46" s="2">
+        <v>93238</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D46" s="2">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="16">
+      <c r="A47" s="2">
+        <v>93390</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D47" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="16">
+      <c r="A48" s="2">
+        <v>93241</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D48" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="16">
+      <c r="A49" s="2">
+        <v>93203</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D49" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="16">
+      <c r="A50" s="2">
+        <v>93524</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D50" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="16">
+      <c r="A51" s="2">
+        <v>93250</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D51" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="16">
+      <c r="A52" s="2">
+        <v>93205</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D52" s="2">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="16">
+      <c r="A53" s="2">
+        <v>93249</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D53" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="16">
+      <c r="A54" s="2">
+        <v>93243</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D54" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="16">
+      <c r="A55" s="2">
+        <v>93226</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D55" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="16">
+      <c r="A56" s="2">
+        <v>93280</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D56" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="16">
+      <c r="A57" s="2">
+        <v>93386</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D57" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="16">
+      <c r="A58" s="2">
+        <v>93276</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D58" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="16">
+      <c r="A59" s="2">
+        <v>93388</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D59" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="16">
+      <c r="A60" s="2">
+        <v>93387</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D60" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="16">
+      <c r="A61" s="2">
+        <v>93505</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D61" s="2">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="16">
+      <c r="A62" s="2">
+        <v>93285</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D62" s="2">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="16">
+      <c r="A63" s="2">
+        <v>93283</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D63" s="2">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="16">
+      <c r="A64" s="2">
+        <v>93502</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D64" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="16">
+      <c r="A65" s="2">
+        <v>93504</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D65" s="2">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="16">
+      <c r="A66" s="2">
+        <v>93501</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D66" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="16">
+      <c r="A67" s="2">
+        <v>93216</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D67" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="16">
+      <c r="A68" s="2">
+        <v>93268</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D68" s="2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="16">
+      <c r="A69" s="2">
+        <v>93263</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D69" s="2">
+        <v>661</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>